<commit_message>
Completed all the plots. Please check and review.
</commit_message>
<xml_diff>
--- a/data_birth_combined.xlsx
+++ b/data_birth_combined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vishalsharma/Downloads/hs501/HS501-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F37C43B-F8AC-1444-8AA8-F5CE8537BC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74020CD-E8F3-5540-9043-B3B793ABA91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,79 +25,79 @@
     <t>state</t>
   </si>
   <si>
-    <t>andhrapradesh</t>
-  </si>
-  <si>
-    <t>arunachalpradesh</t>
-  </si>
-  <si>
-    <t>assam</t>
-  </si>
-  <si>
-    <t>bihar</t>
-  </si>
-  <si>
-    <t>delhi</t>
-  </si>
-  <si>
-    <t>goa</t>
-  </si>
-  <si>
-    <t>gujarat</t>
-  </si>
-  <si>
-    <t>haryana</t>
-  </si>
-  <si>
-    <t>himachalpradesh</t>
-  </si>
-  <si>
-    <t>jammu&amp;kashmir</t>
-  </si>
-  <si>
-    <t>karnataka</t>
-  </si>
-  <si>
-    <t>kerala</t>
-  </si>
-  <si>
-    <t>madhyapradesh</t>
-  </si>
-  <si>
-    <t>maharashtra</t>
-  </si>
-  <si>
-    <t>manipur</t>
-  </si>
-  <si>
-    <t>meghalaya</t>
-  </si>
-  <si>
-    <t>mizoram</t>
-  </si>
-  <si>
-    <t>nagaland</t>
-  </si>
-  <si>
-    <t>odisha</t>
-  </si>
-  <si>
-    <t>punjab</t>
-  </si>
-  <si>
-    <t>rajasthan</t>
-  </si>
-  <si>
-    <t>tamilnadu</t>
-  </si>
-  <si>
-    <t>tripura</t>
-  </si>
-  <si>
-    <t>uttarpradesh</t>
-  </si>
-  <si>
-    <t>westbengal</t>
+    <t>Arunachal Pradesh</t>
+  </si>
+  <si>
+    <t>Andhra Pradesh</t>
+  </si>
+  <si>
+    <t>Assam</t>
+  </si>
+  <si>
+    <t>Bihar</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+  <si>
+    <t>Gujarat</t>
+  </si>
+  <si>
+    <t>Haryana</t>
+  </si>
+  <si>
+    <t>Himachal Pradesh</t>
+  </si>
+  <si>
+    <t>Jammu &amp; Kashmir</t>
+  </si>
+  <si>
+    <t>Karnatka</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>Madhya Pradesh</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>Manipur</t>
+  </si>
+  <si>
+    <t>Meghalya</t>
+  </si>
+  <si>
+    <t>Mizoram</t>
+  </si>
+  <si>
+    <t>Nagaland</t>
+  </si>
+  <si>
+    <t>Odisha</t>
+  </si>
+  <si>
+    <t>Punjab</t>
+  </si>
+  <si>
+    <t>Rajasthan</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>Tripura</t>
+  </si>
+  <si>
+    <t>Uttar Pradesh</t>
+  </si>
+  <si>
+    <t>West Bengal</t>
   </si>
 </sst>
 </file>
@@ -463,11 +463,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1048576"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -491,7 +494,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>11517</v>
@@ -511,7 +514,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>2728</v>

</xml_diff>